<commit_message>
Added Vizgen and MERSCOPE instruments
Closes #65
</commit_message>
<xml_diff>
--- a/merfish/latest/merfish.xlsx
+++ b/merfish/latest/merfish.xlsx
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="350">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -677,6 +677,12 @@
     <t>https://identifiers.org/RRID:SCR_023607</t>
   </si>
   <si>
+    <t>Vizgen</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026274</t>
+  </si>
+  <si>
     <t>Standard BioTools (Fluidigm)</t>
   </si>
   <si>
@@ -1034,6 +1040,12 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
+    <t>MERSCOPE</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000404</t>
+  </si>
+  <si>
     <t>NextSeq 2000</t>
   </si>
   <si>
@@ -1076,6 +1088,12 @@
     <t>https://identifiers.org/RRID:SCR_023909</t>
   </si>
   <si>
+    <t>MERSCOPE Ultra</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026273</t>
+  </si>
+  <si>
     <t>Axio Scan.Z1</t>
   </si>
   <si>
@@ -1313,7 +1331,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-01-08T12:49:22-08:00</t>
+    <t>2025-01-13T10:06:48-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1490,91 +1508,91 @@
         <v>116</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>335</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2">
@@ -1582,7 +1600,7 @@
         <v>62</v>
       </c>
       <c r="AJ2" t="s" s="37">
-        <v>336</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -1597,10 +1615,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$23</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$24</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$52</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$54</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1690,10 +1708,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -1711,10 +1729,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -1732,10 +1750,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -1753,18 +1771,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -1782,106 +1800,106 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>307</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>313</v>
+        <v>319</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>325</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>327</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -1928,16 +1946,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>342</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2">
@@ -1945,13 +1963,13 @@
         <v>62</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>343</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -2442,7 +2460,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2632,6 +2650,14 @@
         <v>162</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>163</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>164</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2639,7 +2665,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2647,418 +2673,434 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>270</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>272</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3076,42 +3118,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -3129,26 +3171,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3166,18 +3208,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "chemistry kit" field
Closes #104
</commit_message>
<xml_diff>
--- a/merfish/latest/merfish.xlsx
+++ b/merfish/latest/merfish.xlsx
@@ -21,7 +21,8 @@
     <sheet name="probe_hybridization_time_unit" r:id="rId15" sheetId="13"/>
     <sheet name="oligo_probe_panel" r:id="rId16" sheetId="14"/>
     <sheet name="is_custom_probes_used" r:id="rId17" sheetId="15"/>
-    <sheet name=".metadata" r:id="rId18" sheetId="16"/>
+    <sheet name="chemistry_kit" r:id="rId18" sheetId="16"/>
+    <sheet name=".metadata" r:id="rId19" sheetId="17"/>
   </sheets>
 </workbook>
 </file>
@@ -278,6 +279,14 @@
     </comment>
     <comment ref="AJ1" authorId="1">
       <text>
+        <t>(Required) The chemistry kit that contains specific set of reagents, probes, and
+protocols used to perform the assay. This typically includes assay-specific
+probes, buffers, and other chemical components required for hybridization,
+amplification, and imaging.</t>
+      </text>
+    </comment>
+    <comment ref="AK1" authorId="1">
+      <text>
         <t>(Required) The string that serves as the definitive identifier for the metadata
 schema version and is readily interpretable by computers for data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
@@ -288,7 +297,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="427">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -308,6 +317,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000195</t>
   </si>
   <si>
+    <t>Olink</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000441</t>
+  </si>
+  <si>
     <t>SNARE-seq2</t>
   </si>
   <si>
@@ -344,6 +359,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
   </si>
   <si>
+    <t>FACS</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000440</t>
+  </si>
+  <si>
     <t>Xenium</t>
   </si>
   <si>
@@ -446,6 +467,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
   </si>
   <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -683,6 +710,18 @@
     <t>https://identifiers.org/RRID:SCR_023607</t>
   </si>
   <si>
+    <t>Complete Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027007</t>
+  </si>
+  <si>
+    <t>3DHISTECH</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027042</t>
+  </si>
+  <si>
     <t>GE Healthcare</t>
   </si>
   <si>
@@ -797,12 +836,24 @@
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>Cytek Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027071</t>
+  </si>
+  <si>
     <t>10x Genomics</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023672</t>
   </si>
   <si>
+    <t>Microscopes International</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027094</t>
+  </si>
+  <si>
     <t>Hamamatsu</t>
   </si>
   <si>
@@ -836,6 +887,12 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>Pannoramic MIDI II Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024834</t>
+  </si>
+  <si>
     <t>Not applicable</t>
   </si>
   <si>
@@ -944,6 +1001,12 @@
     <t>https://identifiers.org/RRID:SCR_019916</t>
   </si>
   <si>
+    <t>uScopeHXII-20</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027101</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -1022,6 +1085,12 @@
     <t>https://identifiers.org/RRID:SCR_016381</t>
   </si>
   <si>
+    <t>Axio Zoom.V16</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027090</t>
+  </si>
+  <si>
     <t>Digital Spatial Profiler</t>
   </si>
   <si>
@@ -1058,6 +1127,12 @@
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
+    <t>Cytek Northern Lights</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027072</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -1172,6 +1247,12 @@
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
+    <t>solariX</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027095</t>
+  </si>
+  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -1184,6 +1265,12 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>Biomark HD</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_022658</t>
+  </si>
+  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -1208,6 +1295,12 @@
     <t>https://identifiers.org/RRID:SCR_020927</t>
   </si>
   <si>
+    <t>Juno System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027198</t>
+  </si>
+  <si>
     <t>Q Exactive HF</t>
   </si>
   <si>
@@ -1346,6 +1439,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000383</t>
   </si>
   <si>
+    <t>10x Genomics; Xenium Mouse Multi-Tissue Atlassing Panel; PN 1000627</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000442</t>
+  </si>
+  <si>
     <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
   </si>
   <si>
@@ -1394,6 +1493,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000376</t>
   </si>
   <si>
+    <t>NanoString Technologies; CosMx Human Immuno-Oncology Panel (Protein, 64 Plex); PN CMX-H-IOP-64P-P</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000436</t>
+  </si>
+  <si>
     <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome, 4 rxns x 1 BC; PN 1000474</t>
   </si>
   <si>
@@ -1412,6 +1517,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000430</t>
   </si>
   <si>
+    <t>NanoString Technologies; CosMx Mouse Neuroscience Panel (Protein, 64 Plex); PN CMX-M-Neuro-64P-P</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000437</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 16 rxns; PN 1000420</t>
   </si>
   <si>
@@ -1439,6 +1550,9 @@
     <t>number_of_additional_stains</t>
   </si>
   <si>
+    <t>chemistry_kit</t>
+  </si>
+  <si>
     <t>metadata_schema_id</t>
   </si>
   <si>
@@ -1457,7 +1571,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-05-12T10:18:23-07:00</t>
+    <t>2025-07-16T11:41:27-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1516,7 +1630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
       <alignment horizontal="center"/>
@@ -1557,6 +1671,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -1567,7 +1682,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1608,7 +1723,8 @@
     <col min="33" max="33" style="34" width="19.23828125" customWidth="true" bestFit="true"/>
     <col min="34" max="34" style="35" width="13.33984375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" style="36" width="22.95703125" customWidth="true" bestFit="true"/>
-    <col min="36" max="36" style="37" width="16.91796875" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" style="37" width="11.140625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" style="38" width="16.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1625,114 +1741,117 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>311</v>
+        <v>339</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>322</v>
+        <v>350</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>323</v>
+        <v>351</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>324</v>
+        <v>352</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>325</v>
+        <v>353</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>326</v>
+        <v>354</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>327</v>
+        <v>355</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>332</v>
+        <v>360</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>333</v>
+        <v>361</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>334</v>
+        <v>362</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>335</v>
+        <v>363</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>336</v>
+        <v>364</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>337</v>
+        <v>365</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>338</v>
+        <v>366</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>339</v>
+        <v>367</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>340</v>
+        <v>368</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>341</v>
+        <v>369</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>342</v>
+        <v>370</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>343</v>
+        <v>371</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>376</v>
+        <v>410</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>377</v>
+        <v>411</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>378</v>
+        <v>412</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>379</v>
+        <v>413</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>380</v>
+        <v>414</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>381</v>
+        <v>415</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>382</v>
+        <v>416</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>383</v>
+        <v>417</v>
+      </c>
+      <c r="AK1" t="s" s="1">
+        <v>418</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>64</v>
-      </c>
-      <c r="AJ2" t="s" s="37">
-        <v>384</v>
+        <v>70</v>
+      </c>
+      <c r="AK2" t="s" s="38">
+        <v>419</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="25">
+  <dataValidations count="26">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$41</formula1>
+      <formula1>'dataset_type'!$A$1:$A$44</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1741,10 +1860,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$26</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$68</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$75</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1804,7 +1923,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AB2:AB1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$16</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$19</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AC2:AC1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -1816,6 +1935,9 @@
     <dataValidation type="whole" operator="between" sqref="AI2:AI1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-2147483648</formula1>
       <formula2>2147483647</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="AJ2:AJ1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'chemistry_kit'!$A$1:$A$1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1834,10 +1956,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>320</v>
+        <v>348</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>321</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -1855,10 +1977,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>320</v>
+        <v>348</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>321</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -1876,10 +1998,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>320</v>
+        <v>348</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>321</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -1897,18 +2019,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>312</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>313</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>320</v>
+        <v>348</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>321</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -1918,7 +2040,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1926,130 +2048,154 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>344</v>
+        <v>372</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>345</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>346</v>
+        <v>374</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>347</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>348</v>
+        <v>376</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>349</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>350</v>
+        <v>378</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>351</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>352</v>
+        <v>380</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>353</v>
+        <v>381</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>354</v>
+        <v>382</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>355</v>
+        <v>383</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>356</v>
+        <v>384</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>357</v>
+        <v>385</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>358</v>
+        <v>386</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>359</v>
+        <v>387</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>360</v>
+        <v>388</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>361</v>
+        <v>389</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>362</v>
+        <v>390</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>363</v>
+        <v>391</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>364</v>
+        <v>392</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>365</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>366</v>
+        <v>394</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>367</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>368</v>
+        <v>396</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>369</v>
+        <v>397</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>370</v>
+        <v>398</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>371</v>
+        <v>399</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>372</v>
+        <v>400</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>373</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>374</v>
+        <v>402</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>375</v>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>404</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>406</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>408</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -2067,12 +2213,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2081,6 +2227,27 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>386</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>387</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2096,30 +2263,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>385</v>
+        <v>420</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>386</v>
+        <v>421</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>388</v>
+        <v>423</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>390</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>387</v>
+        <v>422</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>389</v>
+        <v>424</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>391</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -2129,7 +2296,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2461,6 +2628,30 @@
       </c>
       <c r="B41" t="s" s="0">
         <v>85</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2478,130 +2669,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2619,12 +2810,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2634,7 +2825,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2642,210 +2833,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>174</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>181</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>183</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>185</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>187</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2855,7 +3078,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2863,546 +3086,602 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>177</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>179</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>181</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>183</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>185</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>187</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>189</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>191</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>193</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>195</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>197</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>199</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>201</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>203</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>205</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>207</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>209</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>211</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>215</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>219</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>221</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>223</v>
+        <v>237</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>225</v>
+        <v>239</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>227</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>229</v>
+        <v>243</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>231</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>233</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>235</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>237</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>239</v>
+        <v>253</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>241</v>
+        <v>255</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>243</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>247</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>249</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>251</v>
+        <v>265</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>253</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>255</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>257</v>
+        <v>271</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>259</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>261</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>263</v>
+        <v>277</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>265</v>
+        <v>279</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>267</v>
+        <v>281</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>269</v>
+        <v>283</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>271</v>
+        <v>285</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>273</v>
+        <v>287</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>275</v>
+        <v>289</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>277</v>
+        <v>291</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>279</v>
+        <v>293</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>281</v>
+        <v>295</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>283</v>
+        <v>297</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>285</v>
+        <v>299</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>287</v>
+        <v>301</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>289</v>
+        <v>303</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>291</v>
+        <v>305</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>149</v>
+        <v>306</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>150</v>
+        <v>307</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>292</v>
+        <v>308</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>293</v>
+        <v>309</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>294</v>
+        <v>310</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>295</v>
+        <v>311</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>296</v>
+        <v>312</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>297</v>
+        <v>313</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>298</v>
+        <v>159</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>299</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>300</v>
+        <v>314</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>301</v>
+        <v>315</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>303</v>
+        <v>317</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>306</v>
+        <v>320</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>307</v>
+        <v>321</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>308</v>
+        <v>322</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>309</v>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>324</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>326</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>328</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>330</v>
+      </c>
+      <c r="B72" t="s" s="0">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>332</v>
+      </c>
+      <c r="B73" t="s" s="0">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>334</v>
+      </c>
+      <c r="B74" t="s" s="0">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>336</v>
+      </c>
+      <c r="B75" t="s" s="0">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -3420,42 +3699,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>312</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>313</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>314</v>
+        <v>342</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>315</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>316</v>
+        <v>344</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>317</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>318</v>
+        <v>346</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>319</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>320</v>
+        <v>348</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>321</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -3473,26 +3752,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>314</v>
+        <v>342</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>315</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>316</v>
+        <v>344</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>317</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>318</v>
+        <v>346</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>319</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -3510,18 +3789,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>328</v>
+        <v>356</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>329</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>330</v>
+        <v>358</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>331</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>